<commit_message>
Created Random Compression Generating Algorithm
Mostly works, however on decompression the decompressed graph has some repeated nodes...not 100% why...needs to be looked into.

All raw data is included in the algorithms/generating_random_compressed_results folder
</commit_message>
<xml_diff>
--- a/algorithms/bipartite_and_topsort_tests/fixed_bipartite/Fixed Bipartite Averages.xlsx
+++ b/algorithms/bipartite_and_topsort_tests/fixed_bipartite/Fixed Bipartite Averages.xlsx
@@ -387,11 +387,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="665967584"/>
-        <c:axId val="637298560"/>
+        <c:axId val="-1583765216"/>
+        <c:axId val="-1583767760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="665967584"/>
+        <c:axId val="-1583765216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,12 +508,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="637298560"/>
+        <c:crossAx val="-1583767760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="637298560"/>
+        <c:axId val="-1583767760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +631,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="665967584"/>
+        <c:crossAx val="-1583765216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1055,11 +1055,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="670155856"/>
-        <c:axId val="666622816"/>
+        <c:axId val="-1580855680"/>
+        <c:axId val="-1652835056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="670155856"/>
+        <c:axId val="-1580855680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1176,12 +1176,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="666622816"/>
+        <c:crossAx val="-1652835056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="666622816"/>
+        <c:axId val="-1652835056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,7 +1299,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="670155856"/>
+        <c:crossAx val="-1580855680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1641,11 +1641,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="666279408"/>
-        <c:axId val="669645760"/>
+        <c:axId val="-1583447232"/>
+        <c:axId val="-1583444112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="666279408"/>
+        <c:axId val="-1583447232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,12 +1762,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="669645760"/>
+        <c:crossAx val="-1583444112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="669645760"/>
+        <c:axId val="-1583444112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1885,7 +1885,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="666279408"/>
+        <c:crossAx val="-1583447232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4559,7 +4559,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H10"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4838,8 +4838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Randomly compressed graph method added
New function allows for a randomly compressed graph to be made. Development still needs to done to control for compression ratio. Last commit. :(
</commit_message>
<xml_diff>
--- a/algorithms/bipartite_and_topsort_tests/fixed_bipartite/Fixed Bipartite Averages.xlsx
+++ b/algorithms/bipartite_and_topsort_tests/fixed_bipartite/Fixed Bipartite Averages.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="15">
   <si>
     <t>100 Nodes</t>
   </si>
@@ -76,15 +76,34 @@
   <si>
     <t>200 Nodes</t>
   </si>
+  <si>
+    <t>`</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,13 +126,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -161,11 +184,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Bipartite </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>on </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Uncompressed</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Graph</a:t>
+              <a:t> Highly Compressible Graph</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -387,11 +418,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1583765216"/>
-        <c:axId val="-1583767760"/>
+        <c:axId val="-237061456"/>
+        <c:axId val="-238152864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1583765216"/>
+        <c:axId val="-237061456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,12 +539,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1583767760"/>
+        <c:crossAx val="-238152864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1583767760"/>
+        <c:axId val="-238152864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +662,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1583765216"/>
+        <c:crossAx val="-237061456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -747,7 +778,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Compression Aware Algorithm</a:t>
+              <a:t>Compression Aware Bipartite Algorithm</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1055,11 +1086,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1580855680"/>
-        <c:axId val="-1652835056"/>
+        <c:axId val="-195686656"/>
+        <c:axId val="-195682896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1580855680"/>
+        <c:axId val="-195686656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1176,12 +1207,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1652835056"/>
+        <c:crossAx val="-195682896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1652835056"/>
+        <c:axId val="-195682896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,7 +1330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1580855680"/>
+        <c:crossAx val="-195686656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1641,11 +1672,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1583447232"/>
-        <c:axId val="-1583444112"/>
+        <c:axId val="-195660944"/>
+        <c:axId val="-195657184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1583447232"/>
+        <c:axId val="-195660944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,12 +1793,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1583444112"/>
+        <c:crossAx val="-195657184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1583444112"/>
+        <c:axId val="-195657184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1885,7 +1916,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1583447232"/>
+        <c:crossAx val="-195660944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4836,26 +4867,26 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H73"/>
+  <dimension ref="A2:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F2" t="str">
         <f>Sheet1!A3</f>
         <v xml:space="preserve">Time for perfect normal bippartite algorithm: </v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4872,7 +4903,7 @@
         <v>6.1929702758789004E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -4889,7 +4920,7 @@
         <v>2.9224014282226402E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -4906,7 +4937,7 @@
         <v>5.3441572189331002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4922,8 +4953,11 @@
         <f>Sheet4!I3</f>
         <v>9.1229724884033206E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4940,7 +4974,7 @@
         <v>0.1422957897186278</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4957,18 +4991,18 @@
         <v>0.21809296607971002</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F11" t="str">
         <f>Sheet1!A4</f>
         <v xml:space="preserve">Time for normal bippartite run using compression aware algorithm: </v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F13">
         <f>Sheet1!G4</f>
         <v>4.7996997833251898E-2</v>
@@ -4982,7 +5016,7 @@
         <v>9.5993995666503792E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F14">
         <f>Sheet2!G4</f>
         <v>0.2142915725708</v>
@@ -4996,7 +5030,7 @@
         <v>4.2858314514160001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F15">
         <f>Sheet3!G4</f>
         <v>0.42409372329711897</v>
@@ -5010,7 +5044,7 @@
         <v>8.4818744659423795E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F16">
         <f>Sheet4!G4</f>
         <v>0.73574590682983398</v>
@@ -5594,6 +5628,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>